<commit_message>
added TA to the doc
</commit_message>
<xml_diff>
--- a/UiPath.xlsx
+++ b/UiPath.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miliansolberg/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miliansolberg/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DE2DE2-408A-0640-B8E3-9AD69D938C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864A8E77-28AD-5B45-8577-CFC0D03B65D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{EC6D5C9F-7749-374B-BD09-7D3930FC177D}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Model" sheetId="2" r:id="rId1"/>
     <sheet name="Main" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -203,7 +203,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -266,10 +266,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -298,15 +298,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>527119</xdr:colOff>
+      <xdr:colOff>349319</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>26220</xdr:rowOff>
+      <xdr:rowOff>77020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>166057</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>826457</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>11018</xdr:rowOff>
+      <xdr:rowOff>61818</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -329,8 +329,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15575936" y="2074607"/>
-          <a:ext cx="7668616" cy="8178346"/>
+          <a:off x="15462319" y="2109020"/>
+          <a:ext cx="7792338" cy="8112798"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -341,15 +341,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>248138</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>425938</xdr:colOff>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>82700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>187559</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>365359</xdr:colOff>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>60568</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -380,8 +380,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2938353" y="7047216"/>
-          <a:ext cx="10591034" cy="6327868"/>
+          <a:off x="15538938" y="10852300"/>
+          <a:ext cx="10607421" cy="6277068"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -396,6 +396,50 @@
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Bilde 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A775BC3-BA40-941D-850A-523B81710D23}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="7112000"/>
+          <a:ext cx="13563600" cy="8255000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -702,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D611AFC-0200-8646-B72F-3425955E55E0}">
   <dimension ref="A2:Z29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
+      <selection activeCell="Z29" sqref="Z29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1105,39 +1149,39 @@
         <v>37</v>
       </c>
       <c r="C15" s="1">
-        <f>C6/C4</f>
+        <f t="shared" ref="C15:K15" si="4">C6/C4</f>
         <v>0.87941964404127215</v>
       </c>
       <c r="D15" s="1">
-        <f>D6/D4</f>
+        <f t="shared" si="4"/>
         <v>0.89454425439099994</v>
       </c>
       <c r="E15" s="1">
-        <f>E6/E4</f>
+        <f t="shared" si="4"/>
         <v>0.88196674564970912</v>
       </c>
       <c r="F15" s="1">
-        <f>F6/F4</f>
+        <f t="shared" si="4"/>
         <v>0.90313409500901987</v>
       </c>
       <c r="G15" s="1">
-        <f>G6/G4</f>
+        <f t="shared" si="4"/>
         <v>0.7368124285108234</v>
       </c>
       <c r="H15" s="1">
-        <f>H6/H4</f>
+        <f t="shared" si="4"/>
         <v>0.81795305875072244</v>
       </c>
       <c r="I15" s="1">
-        <f>I6/I4</f>
+        <f t="shared" si="4"/>
         <v>0.80481486848779071</v>
       </c>
       <c r="J15" s="1">
-        <f>J6/J4</f>
+        <f t="shared" si="4"/>
         <v>0.85790719991163211</v>
       </c>
       <c r="K15" s="1">
-        <f>K6/K4</f>
+        <f t="shared" si="4"/>
         <v>0.81631070813576756</v>
       </c>
       <c r="L15" s="1"/>
@@ -1187,15 +1231,15 @@
         <v>73.899999999999977</v>
       </c>
       <c r="I18">
-        <f t="shared" ref="I18:K18" si="4">I17-H17</f>
+        <f t="shared" ref="I18:K18" si="5">I17-H17</f>
         <v>91.899999999999977</v>
       </c>
       <c r="J18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>106.89999999999998</v>
       </c>
       <c r="K18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>51.800000000000068</v>
       </c>
     </row>
@@ -1301,19 +1345,19 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2">
-        <f t="shared" ref="H25:K25" si="5">H27*H26</f>
+        <f t="shared" ref="H25:K25" si="6">H27*H26</f>
         <v>32907000</v>
       </c>
       <c r="I25" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>26692243.600000001</v>
       </c>
       <c r="J25" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>19606413</v>
       </c>
       <c r="K25" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10025187</v>
       </c>
     </row>

</xml_diff>